<commit_message>
Update 02. AUTOMATION SOLUTIOS ( AUTOSOL) - EVALUACION FINANCIERA.xlsx
</commit_message>
<xml_diff>
--- a/Documents/02. AUTOMATION SOLUTIOS ( AUTOSOL) - EVALUACION FINANCIERA.xlsx
+++ b/Documents/02. AUTOMATION SOLUTIOS ( AUTOSOL) - EVALUACION FINANCIERA.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\GitHub\ausol-apm.github.io\project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\GitHub\ausol-apm.github.io\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58B3976-D2CF-4806-98EB-9B107F1E3CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EFC09C-FCE4-432E-8A70-83A968BCCFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proyección ventas" sheetId="2" r:id="rId1"/>
-    <sheet name="Evaluación fianciera" sheetId="3" r:id="rId2"/>
+    <sheet name="Evaluación financiera" sheetId="3" r:id="rId2"/>
+    <sheet name="Justificación Costos" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Evaluación fianciera'!$A$1:$O$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Evaluación financiera'!$A$1:$O$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -146,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>PRODUCTO</t>
   </si>
@@ -337,12 +338,54 @@
   <si>
     <t>AUTOMATION SOLUTIOS ( AUSOL) - EVALUACION FINANCIERA</t>
   </si>
+  <si>
+    <t>Costos promedio para fabricación de un juguete</t>
+  </si>
+  <si>
+    <t>Plástico de inyección</t>
+  </si>
+  <si>
+    <t>Bolsa de empaque</t>
+  </si>
+  <si>
+    <t>Caja de empaque</t>
+  </si>
+  <si>
+    <t>Pintura</t>
+  </si>
+  <si>
+    <t>Costo promedio de los juguetes</t>
+  </si>
+  <si>
+    <t>Porcentaje de materia prima y empaque respecto al costo de venta promedio del juguete</t>
+  </si>
+  <si>
+    <t>Costo materia prima y empaque</t>
+  </si>
+  <si>
+    <t>Gasto promedio de energía por fabricación de juguete</t>
+  </si>
+  <si>
+    <t>Porcentaje de gasto de energía eléctrica respecto al costo promedio de venta del juguete</t>
+  </si>
+  <si>
+    <t>Costo kV/h para industria en Bogotá</t>
+  </si>
+  <si>
+    <t>Bodega y Mantenimientos</t>
+  </si>
+  <si>
+    <t>Bodega de 300 m cuadrados en zona industrial de bogotá</t>
+  </si>
+  <si>
+    <t>Mantenimiento mensual estimado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -352,8 +395,9 @@
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="[$$-240A]\ #,##0.00"/>
     <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="173" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,6 +479,22 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -468,7 +528,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -554,6 +614,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -562,7 +635,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -667,6 +740,44 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3649,12 +3760,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Evaluación fianciera'!$C$17</c:f>
+              <c:f>'Evaluación financiera'!$C$17</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-866000000</c:v>
+                  <c:v>-967883006.27999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3680,12 +3791,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Evaluación fianciera'!$D$17</c:f>
+              <c:f>'Evaluación financiera'!$D$17</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>174125466.66666669</c:v>
+                  <c:v>171005466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3711,12 +3822,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Evaluación fianciera'!$E$17</c:f>
+              <c:f>'Evaluación financiera'!$E$17</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>174125466.66666669</c:v>
+                  <c:v>171005466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3742,12 +3853,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Evaluación fianciera'!$F$17</c:f>
+              <c:f>'Evaluación financiera'!$F$17</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>174125466.66666669</c:v>
+                  <c:v>171005466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3773,12 +3884,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Evaluación fianciera'!$G$17</c:f>
+              <c:f>'Evaluación financiera'!$G$17</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>524342000</c:v>
+                  <c:v>521222000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3804,12 +3915,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Evaluación fianciera'!$H$17</c:f>
+              <c:f>'Evaluación financiera'!$H$17</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>174125466.66666669</c:v>
+                  <c:v>171005466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3837,12 +3948,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Evaluación fianciera'!$I$17</c:f>
+              <c:f>'Evaluación financiera'!$I$17</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>433376666.66666675</c:v>
+                  <c:v>430256666.66666675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3870,12 +3981,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Evaluación fianciera'!$J$17</c:f>
+              <c:f>'Evaluación financiera'!$J$17</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>433376666.66666675</c:v>
+                  <c:v>430256666.66666675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3903,12 +4014,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Evaluación fianciera'!$K$17</c:f>
+              <c:f>'Evaluación financiera'!$K$17</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>174125466.66666669</c:v>
+                  <c:v>171005466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3936,12 +4047,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Evaluación fianciera'!$L$17</c:f>
+              <c:f>'Evaluación financiera'!$L$17</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>174125466.66666669</c:v>
+                  <c:v>171005466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3969,12 +4080,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Evaluación fianciera'!$M$17</c:f>
+              <c:f>'Evaluación financiera'!$M$17</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>342411333.33333337</c:v>
+                  <c:v>339291333.33333337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4002,12 +4113,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Evaluación fianciera'!$N$17</c:f>
+              <c:f>'Evaluación financiera'!$N$17</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>174125466.66666669</c:v>
+                  <c:v>171005466.66666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4036,12 +4147,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Evaluación fianciera'!$O$17</c:f>
+              <c:f>'Evaluación financiera'!$O$17</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* "-"??\ _€_-;_-@_-</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1343030000</c:v>
+                  <c:v>1339910000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7407,7 +7518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C25875F-8E18-430B-8568-E6400B7C666D}">
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="M69" sqref="M69"/>
     </sheetView>
   </sheetViews>
@@ -8499,7 +8610,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="str">
-        <f t="shared" ref="A49:D62" si="11">A2</f>
+        <f t="shared" ref="A50:D62" si="11">A2</f>
         <v>Mes</v>
       </c>
       <c r="B50" s="22" t="str">
@@ -8755,8 +8866,8 @@
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9242,56 +9353,56 @@
         <v>29</v>
       </c>
       <c r="C12" s="1">
-        <f>10*1400000*'Proyección ventas'!L3</f>
-        <v>28000000</v>
+        <f>(10*1400000+2400000)*'Proyección ventas'!L3</f>
+        <v>32800000</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" ref="D12:O12" si="13">+$C$12</f>
-        <v>28000000</v>
+        <v>32800000</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="13"/>
-        <v>28000000</v>
+        <v>32800000</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="13"/>
-        <v>28000000</v>
+        <v>32800000</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="13"/>
-        <v>28000000</v>
+        <v>32800000</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="13"/>
-        <v>28000000</v>
+        <v>32800000</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="13"/>
-        <v>28000000</v>
+        <v>32800000</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="13"/>
-        <v>28000000</v>
+        <v>32800000</v>
       </c>
       <c r="K12" s="1">
         <f t="shared" si="13"/>
-        <v>28000000</v>
+        <v>32800000</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" si="13"/>
-        <v>28000000</v>
+        <v>32800000</v>
       </c>
       <c r="M12" s="1">
         <f t="shared" si="13"/>
-        <v>28000000</v>
+        <v>32800000</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="13"/>
-        <v>28000000</v>
+        <v>32800000</v>
       </c>
       <c r="O12" s="1">
         <f t="shared" si="13"/>
-        <v>28000000</v>
+        <v>32800000</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -9357,51 +9468,51 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" ref="D14:O14" si="15">+D7-D9-D12-D13-D10</f>
-        <v>267885333.33333337</v>
+        <v>263085333.33333337</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="15"/>
-        <v>267885333.33333337</v>
+        <v>263085333.33333337</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="15"/>
-        <v>267885333.33333337</v>
+        <v>263085333.33333337</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="15"/>
-        <v>806680000</v>
+        <v>801880000</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="15"/>
-        <v>267885333.33333337</v>
+        <v>263085333.33333337</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="15"/>
-        <v>666733333.33333349</v>
+        <v>661933333.33333349</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="15"/>
-        <v>666733333.33333349</v>
+        <v>661933333.33333349</v>
       </c>
       <c r="K14" s="1">
         <f t="shared" si="15"/>
-        <v>267885333.33333337</v>
+        <v>263085333.33333337</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="15"/>
-        <v>267885333.33333337</v>
+        <v>263085333.33333337</v>
       </c>
       <c r="M14" s="1">
         <f t="shared" si="15"/>
-        <v>526786666.66666675</v>
+        <v>521986666.66666675</v>
       </c>
       <c r="N14" s="1">
         <f t="shared" si="15"/>
-        <v>267885333.33333337</v>
+        <v>263085333.33333337</v>
       </c>
       <c r="O14" s="1">
         <f t="shared" si="15"/>
-        <v>2066200000</v>
+        <v>2061400000</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -9419,51 +9530,51 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" ref="D16:O16" si="16">+IF(D14&lt;0,0,D14*$C$16)</f>
-        <v>93759866.666666672</v>
+        <v>92079866.666666672</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="16"/>
-        <v>93759866.666666672</v>
+        <v>92079866.666666672</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="16"/>
-        <v>93759866.666666672</v>
+        <v>92079866.666666672</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="16"/>
-        <v>282338000</v>
+        <v>280658000</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="16"/>
-        <v>93759866.666666672</v>
+        <v>92079866.666666672</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="16"/>
-        <v>233356666.66666672</v>
+        <v>231676666.66666672</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="16"/>
-        <v>233356666.66666672</v>
+        <v>231676666.66666672</v>
       </c>
       <c r="K16" s="1">
         <f t="shared" si="16"/>
-        <v>93759866.666666672</v>
+        <v>92079866.666666672</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" si="16"/>
-        <v>93759866.666666672</v>
+        <v>92079866.666666672</v>
       </c>
       <c r="M16" s="1">
         <f t="shared" si="16"/>
-        <v>184375333.33333334</v>
+        <v>182695333.33333334</v>
       </c>
       <c r="N16" s="1">
         <f t="shared" si="16"/>
-        <v>93759866.666666672</v>
+        <v>92079866.666666672</v>
       </c>
       <c r="O16" s="1">
         <f t="shared" si="16"/>
-        <v>723170000</v>
+        <v>721490000</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -9473,55 +9584,55 @@
       <c r="B17" s="13"/>
       <c r="C17" s="13">
         <f>+B18+B19</f>
-        <v>-866000000</v>
+        <v>-967883006.27999997</v>
       </c>
       <c r="D17" s="13">
         <f t="shared" ref="D17:O17" si="17">+D14-D16</f>
-        <v>174125466.66666669</v>
+        <v>171005466.66666669</v>
       </c>
       <c r="E17" s="13">
         <f t="shared" si="17"/>
-        <v>174125466.66666669</v>
+        <v>171005466.66666669</v>
       </c>
       <c r="F17" s="13">
         <f t="shared" si="17"/>
-        <v>174125466.66666669</v>
+        <v>171005466.66666669</v>
       </c>
       <c r="G17" s="13">
         <f t="shared" si="17"/>
-        <v>524342000</v>
+        <v>521222000</v>
       </c>
       <c r="H17" s="13">
         <f t="shared" si="17"/>
-        <v>174125466.66666669</v>
+        <v>171005466.66666669</v>
       </c>
       <c r="I17" s="13">
         <f t="shared" si="17"/>
-        <v>433376666.66666675</v>
+        <v>430256666.66666675</v>
       </c>
       <c r="J17" s="13">
         <f t="shared" si="17"/>
-        <v>433376666.66666675</v>
+        <v>430256666.66666675</v>
       </c>
       <c r="K17" s="13">
         <f t="shared" si="17"/>
-        <v>174125466.66666669</v>
+        <v>171005466.66666669</v>
       </c>
       <c r="L17" s="13">
         <f t="shared" si="17"/>
-        <v>174125466.66666669</v>
+        <v>171005466.66666669</v>
       </c>
       <c r="M17" s="13">
         <f t="shared" si="17"/>
-        <v>342411333.33333337</v>
+        <v>339291333.33333337</v>
       </c>
       <c r="N17" s="13">
         <f t="shared" si="17"/>
-        <v>174125466.66666669</v>
+        <v>171005466.66666669</v>
       </c>
       <c r="O17" s="13">
         <f t="shared" si="17"/>
-        <v>1343030000</v>
+        <v>1339910000</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -9529,7 +9640,7 @@
         <v>52</v>
       </c>
       <c r="B18" s="1">
-        <v>-850000000</v>
+        <v>-951883006.27999997</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -9547,7 +9658,7 @@
       </c>
       <c r="B20" s="16">
         <f>+NPV($B$23,D17:O17)</f>
-        <v>2963346767.125103</v>
+        <v>2935693422.0193825</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -9556,7 +9667,7 @@
       </c>
       <c r="B21" s="16">
         <f>+B20+B18+B19</f>
-        <v>2097346767.125103</v>
+        <v>1967810415.7393825</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -9565,7 +9676,7 @@
       </c>
       <c r="B22" s="17">
         <f>+IRR(C17:O17)</f>
-        <v>0.29022550276133674</v>
+        <v>0.25834318049856475</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -9600,4 +9711,159 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D468B599-A3E8-4977-B436-DBE6E05B3FE2}">
+  <dimension ref="A1:N10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
+    <col min="13" max="13" width="13.77734375" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="K1" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="57">
+        <f>M2+M3</f>
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="49">
+        <f>SUM(B3:B6)</f>
+        <v>1854</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="50">
+        <f>(SUM('Proyección ventas'!H3:H5)/3)</f>
+        <v>12333.333333333334</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="51">
+        <f>(B2/E2)*100</f>
+        <v>15.032432432432433</v>
+      </c>
+      <c r="K2" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="56"/>
+      <c r="M2" s="54">
+        <f>4000000</f>
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="47">
+        <v>750</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="42"/>
+      <c r="M3" s="57">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="47">
+        <f>100/25</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="47">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A9" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+    </row>
+    <row r="10" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="55">
+        <f>E10*1.21</f>
+        <v>370.0301</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="55">
+        <v>305.81</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="55">
+        <f>(B10/E2)*100</f>
+        <v>3.000244054054054</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>